<commit_message>
modif rang colonne écart
</commit_message>
<xml_diff>
--- a/build/exe.win-amd64-3.8/code_shopping.xlsx
+++ b/build/exe.win-amd64-3.8/code_shopping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiphaine\Documents\scraping_eaugo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC10EE2-AF24-4A2D-9927-2AD324B9C6F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC22967-66E1-4B78-BAEA-1179EE32F69C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{F1B0C1AC-FB7A-4110-BEEE-F669CB1D5F9F}"/>
   </bookViews>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD20CB67-C8C9-4B94-A094-16822D659378}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B52"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -777,116 +777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2">
-        <v>3661238349124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2">
-        <v>3410531531107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="2">
-        <v>3546332710479</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="2">
-        <v>3661238583719</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="2">
-        <v>3410530223300</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="2">
-        <v>3410531554205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="2">
-        <v>3661238583726</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2">
-        <v>3661238349117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="2">
-        <v>3410530521253</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="2">
-        <v>3661238349131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2">
-        <v>3661238568921</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2">
-        <v>3661238568938</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="2">
-        <v>3410531554106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2">
-        <v>3546332310389</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="2">
-        <v>3546332410980</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="2">
-        <v>3546332610670</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="2">
-        <v>3546332631231</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="2">
-        <v>3546332710837</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="2">
-        <v>3546332810421</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="2">
-        <v>3546332810674</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="2">
-        <v>3546332831181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="2">
-        <v>3546338614108</v>
-      </c>
-    </row>
+    <row r="52" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>